<commit_message>
Spatial and temporal visualization
</commit_message>
<xml_diff>
--- a/data/other/calendar.xlsx
+++ b/data/other/calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carle\Documents\GEOTECH\IFGI\DataToKnowledge\research_project\Air-Quality\data\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20FED860-55FB-4F15-901B-60910140F9DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA042FB3-293F-42F6-A745-0145C8AE2F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FA4542DA-D26D-46FC-B0C5-9F644C57F0D9}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>2020-03-18</t>
   </si>
   <si>
-    <t>2020-03-01</t>
-  </si>
-  <si>
     <t>Pre-emergency</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>End restrictions</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,10 +461,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -472,55 +472,55 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>